<commit_message>
Fixed number of cars
</commit_message>
<xml_diff>
--- a/Data/Transport Technology Characteristics.xlsx
+++ b/Data/Transport Technology Characteristics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\NEON-Integrated-Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8259DB-2994-46BC-8E4E-14BD761C097C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C410697D-50CB-4F43-B790-5F278F529E96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9AFF1A54-1272-4A20-A3EF-CBFA1B8A79D5}"/>
   </bookViews>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92654273-2121-465A-9033-66783D7669E0}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1101,7 +1101,7 @@
         <v>7142431</v>
       </c>
       <c r="E2" s="5">
-        <f>D2/$R$2</f>
+        <f t="shared" ref="E2:E7" si="0">D2/$R$2</f>
         <v>0.80839363474266634</v>
       </c>
       <c r="F2" s="8">
@@ -1170,7 +1170,7 @@
         <v>1406856</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E7" si="0">D3/$R$2</f>
+        <f t="shared" si="0"/>
         <v>0.15923058065237572</v>
       </c>
       <c r="F3" s="8">
@@ -1254,7 +1254,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>21136</v>
@@ -1299,7 +1299,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>42</v>
@@ -1344,7 +1344,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>98773</v>

</xml_diff>